<commit_message>
Hasta aquí se guarda el nuevo texto en un archivo nuevo pero sin estilo
</commit_message>
<xml_diff>
--- a/Variables para automatización memorias de calculo.xlsx
+++ b/Variables para automatización memorias de calculo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\root\projects\memcalculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2496C15-773E-4317-A70B-76D7E08434C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C4D0F1-A348-421D-A3BE-BE58FE407C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5D05AEF4-27F9-4C77-8016-BF0321375D48}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Nombre de la variable</t>
   </si>
   <si>
-    <t xml:space="preserve">Valor </t>
-  </si>
-  <si>
     <t>Descripción de la variable</t>
   </si>
   <si>
@@ -263,6 +260,9 @@
   </si>
   <si>
     <t>NameID</t>
+  </si>
+  <si>
+    <t>Valor</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,19 +730,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -760,10 +760,10 @@
         <v>float001</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -771,7 +771,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -781,10 +781,10 @@
         <v>string001</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -792,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5">
         <v>2</v>
@@ -802,10 +802,10 @@
         <v>string002</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -813,7 +813,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5">
         <v>3</v>
@@ -823,7 +823,7 @@
         <v>string003</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="8">
         <v>45323</v>
@@ -834,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
@@ -844,10 +844,10 @@
         <v>string004</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -865,10 +865,10 @@
         <v>int001</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -876,7 +876,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5">
         <v>2</v>
@@ -886,10 +886,10 @@
         <v>int002</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -897,7 +897,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5">
         <v>3</v>
@@ -907,7 +907,7 @@
         <v>int003</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="5">
         <v>132</v>
@@ -918,7 +918,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5">
         <v>5</v>
@@ -928,10 +928,10 @@
         <v>string005</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="5">
         <v>4</v>
@@ -949,7 +949,7 @@
         <v>int004</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="5">
         <v>6</v>
@@ -960,7 +960,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="5">
         <v>6</v>
@@ -970,10 +970,10 @@
         <v>string006</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="5">
         <v>5</v>
@@ -991,7 +991,7 @@
         <v>int005</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="5">
         <v>240</v>
@@ -1002,7 +1002,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="5">
         <v>6</v>
@@ -1012,10 +1012,10 @@
         <v>int006</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="5">
         <v>7</v>
@@ -1033,7 +1033,7 @@
         <v>int007</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F15" s="5">
         <v>10</v>
@@ -1044,7 +1044,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="5">
         <v>7</v>
@@ -1054,10 +1054,10 @@
         <v>string007</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1065,7 +1065,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="5">
         <v>2</v>
@@ -1075,10 +1075,10 @@
         <v>float002</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="5">
         <v>3</v>
@@ -1096,10 +1096,10 @@
         <v>float003</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1107,7 +1107,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="5">
         <v>4</v>
@@ -1117,10 +1117,10 @@
         <v>float004</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1128,7 +1128,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="5">
         <v>5</v>
@@ -1138,10 +1138,10 @@
         <v>float 005</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1149,7 +1149,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="5">
         <v>6</v>
@@ -1159,10 +1159,10 @@
         <v>float006</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1170,7 +1170,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="5">
         <v>8</v>
@@ -1180,7 +1180,7 @@
         <v>int008</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="5">
         <v>6</v>
@@ -1191,7 +1191,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="5">
         <v>9</v>
@@ -1201,7 +1201,7 @@
         <v>int009</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23" s="5">
         <v>10</v>
@@ -1212,7 +1212,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="5">
         <v>10</v>
@@ -1222,7 +1222,7 @@
         <v>int010</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F24" s="5">
         <v>16</v>
@@ -1233,7 +1233,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="5">
         <v>11</v>
@@ -1243,7 +1243,7 @@
         <v>int011</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F25" s="5">
         <v>43</v>
@@ -1254,7 +1254,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="5">
         <v>12</v>
@@ -1264,7 +1264,7 @@
         <v>int012</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F26" s="5">
         <v>258</v>
@@ -1275,7 +1275,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="5">
         <v>7</v>
@@ -1285,18 +1285,18 @@
         <v>float007</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F27" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="5">
         <v>13</v>
@@ -1306,7 +1306,7 @@
         <v>int013</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F28" s="5">
         <v>6</v>
@@ -1317,7 +1317,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="5">
         <v>14</v>
@@ -1327,10 +1327,10 @@
         <v>int014</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1338,7 +1338,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="5">
         <v>15</v>
@@ -1348,7 +1348,7 @@
         <v>int015</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F30" s="5">
         <v>50</v>
@@ -1359,7 +1359,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" s="5">
         <v>16</v>
@@ -1369,7 +1369,7 @@
         <v>int016</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31" s="5">
         <v>10</v>
@@ -1380,7 +1380,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="5">
         <v>1</v>
@@ -1390,10 +1390,10 @@
         <v>tabla 001</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1401,7 +1401,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="5">
         <v>8</v>
@@ -1411,10 +1411,10 @@
         <v>float008</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1422,7 +1422,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34" s="5">
         <v>9</v>
@@ -1432,10 +1432,10 @@
         <v>float009</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35" s="5">
         <v>10</v>
@@ -1453,10 +1453,10 @@
         <v>float010</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" s="5">
         <v>11</v>
@@ -1474,7 +1474,7 @@
         <v>float011</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F36" s="5">
         <v>1</v>
@@ -1485,7 +1485,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37" s="5">
         <v>12</v>
@@ -1495,10 +1495,10 @@
         <v>float 012</v>
       </c>
       <c r="E37" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1506,7 +1506,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C38" s="5">
         <v>17</v>
@@ -1516,7 +1516,7 @@
         <v>int017</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F38" s="5">
         <v>350</v>
@@ -1527,7 +1527,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="5">
         <v>18</v>
@@ -1537,7 +1537,7 @@
         <v>int018</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F39" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
Funcionando funciones para reemplazar texto y tablas, las tablas deben salir de una hoja de excel independiente cada una
</commit_message>
<xml_diff>
--- a/Variables para automatización memorias de calculo.xlsx
+++ b/Variables para automatización memorias de calculo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\root\projects\memcalculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C4D0F1-A348-421D-A3BE-BE58FE407C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F4292B-9473-4DF6-BDFC-5F2B63014147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5D05AEF4-27F9-4C77-8016-BF0321375D48}"/>
+    <workbookView xWindow="4485" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{5D05AEF4-27F9-4C77-8016-BF0321375D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Vars" sheetId="1" r:id="rId1"/>
@@ -269,7 +269,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -710,22 +710,22 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5703125" style="2"/>
+    <col min="4" max="4" width="23.75" style="2" customWidth="1"/>
+    <col min="5" max="5" width="29.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -745,7 +745,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="5" customFormat="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -766,7 +766,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="5" customFormat="1">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -808,7 +808,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -819,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B5,"00",C5)</f>
         <v>string003</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -829,7 +829,7 @@
         <v>45323</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="5" customFormat="1">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -850,7 +850,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="5" customFormat="1">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -871,7 +871,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -892,7 +892,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="5" customFormat="1">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -913,7 +913,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="5" customFormat="1">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -934,7 +934,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="5" customFormat="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -955,7 +955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="5" customFormat="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -976,7 +976,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -997,7 +997,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="5" customFormat="1">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="5" customFormat="1">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="5" customFormat="1" ht="42.75">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="5" customFormat="1">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="5" customFormat="1">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="5" customFormat="1">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="5" customFormat="1">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="5" customFormat="1">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="5" customFormat="1">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="5" customFormat="1" ht="42.75">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="5" customFormat="1">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="5" customFormat="1">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="5" customFormat="1">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="5" customFormat="1">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="5" customFormat="1">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="5" customFormat="1" ht="42.75">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A39" s="5">
         <v>38</v>
       </c>

</xml_diff>